<commit_message>
update tableur create protocole
</commit_message>
<xml_diff>
--- a/modele_protocole.xlsx
+++ b/modele_protocole.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="protocole" sheetId="1" r:id="rId1"/>
@@ -40,15 +40,9 @@
     <t>Type en base de données</t>
   </si>
   <si>
-    <t>Chaîne de caractère</t>
-  </si>
-  <si>
     <t>Liste de choix</t>
   </si>
   <si>
-    <t>Booléen</t>
-  </si>
-  <si>
     <t>Entier</t>
   </si>
   <si>
@@ -59,6 +53,12 @@
   </si>
   <si>
     <t>boolean</t>
+  </si>
+  <si>
+    <t>Chaine de caractere</t>
+  </si>
+  <si>
+    <t>Booleen</t>
   </si>
 </sst>
 </file>
@@ -889,7 +889,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
@@ -1015,8 +1015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1027,7 +1027,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -1035,7 +1035,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -1043,23 +1043,23 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>